<commit_message>
spline dr, still need to fix GOF
</commit_message>
<xml_diff>
--- a/data/incidence_dr_globocan.xlsx
+++ b/data/incidence_dr_globocan.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/st3381_cumc_columbia_edu/Documents/HIRE/CRC Screening Models/NH Calibration US/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/st3381_cumc_columbia_edu/Documents/HIRE/CRC Screening Models/dr-crc-calibration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{35A0E001-2FA2-487A-9E36-68090B21B923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DB4A879-C112-47BD-9E70-55D6897A7B78}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="8_{35A0E001-2FA2-487A-9E36-68090B21B923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B72A00FB-0FBB-4EE4-9067-DA6D58856CB9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{28CE8278-F064-480C-86D8-BD239664EDA6}"/>
+    <workbookView minimized="1" xWindow="34590" yWindow="990" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{28CE8278-F064-480C-86D8-BD239664EDA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Globocan" sheetId="1" r:id="rId1"/>
-    <sheet name="1Y INC" sheetId="2" r:id="rId2"/>
-    <sheet name="DR incidence factor" sheetId="6" r:id="rId3"/>
-    <sheet name="1Y INC US STAGE DIST" sheetId="3" r:id="rId4"/>
-    <sheet name="DR 5y factor" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="1Y INC" sheetId="2" r:id="rId3"/>
+    <sheet name="DR 5y raw" sheetId="10" r:id="rId4"/>
+    <sheet name="DR incidence factor" sheetId="6" r:id="rId5"/>
+    <sheet name="1Y INC US STAGE DIST" sheetId="3" r:id="rId6"/>
+    <sheet name="DR 5y factor" sheetId="4" r:id="rId7"/>
+    <sheet name="HGPS Stage" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Age</t>
   </si>
@@ -160,6 +163,27 @@
   </si>
   <si>
     <t>pD</t>
+  </si>
+  <si>
+    <t>Crude 5y</t>
+  </si>
+  <si>
+    <t>Age start</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Regional</t>
+  </si>
+  <si>
+    <t>Distant</t>
   </si>
 </sst>
 </file>
@@ -4786,16 +4810,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>401955</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>97155</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>81915</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5182,7 +5206,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D3" sqref="D3:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5502,15 +5526,143 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D268217-49AC-4BF2-91C0-A2BF0F60A62A}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <v>113.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>80</v>
+      </c>
+      <c r="B14">
+        <v>125.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5414E684-281C-401D-B84E-2666327A8F20}">
   <dimension ref="A1:V68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V1048576"/>
+      <selection activeCell="C1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" customWidth="1"/>
     <col min="16" max="16" width="11.88671875" customWidth="1"/>
     <col min="17" max="17" width="12.5546875" customWidth="1"/>
@@ -8634,12 +8786,571 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3614669D-D3F9-456B-BF78-87AF377F60A2}">
+  <dimension ref="A1:B68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>37</v>
+      </c>
+      <c r="B19">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>38</v>
+      </c>
+      <c r="B20">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>44</v>
+      </c>
+      <c r="B26">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>46</v>
+      </c>
+      <c r="B28">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>48</v>
+      </c>
+      <c r="B30">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>49</v>
+      </c>
+      <c r="B31">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>50</v>
+      </c>
+      <c r="B32">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>51</v>
+      </c>
+      <c r="B33">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>54</v>
+      </c>
+      <c r="B36">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>55</v>
+      </c>
+      <c r="B37">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>56</v>
+      </c>
+      <c r="B38">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>58</v>
+      </c>
+      <c r="B40">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>59</v>
+      </c>
+      <c r="B41">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>60</v>
+      </c>
+      <c r="B42">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>61</v>
+      </c>
+      <c r="B43">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>62</v>
+      </c>
+      <c r="B44">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>63</v>
+      </c>
+      <c r="B45">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>64</v>
+      </c>
+      <c r="B46">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>65</v>
+      </c>
+      <c r="B47">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>66</v>
+      </c>
+      <c r="B48">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>67</v>
+      </c>
+      <c r="B49">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>68</v>
+      </c>
+      <c r="B50">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>69</v>
+      </c>
+      <c r="B51">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>70</v>
+      </c>
+      <c r="B52">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>71</v>
+      </c>
+      <c r="B53">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>72</v>
+      </c>
+      <c r="B54">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>73</v>
+      </c>
+      <c r="B55">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>74</v>
+      </c>
+      <c r="B56">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>75</v>
+      </c>
+      <c r="B57">
+        <v>113.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>76</v>
+      </c>
+      <c r="B58">
+        <v>113.3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>77</v>
+      </c>
+      <c r="B59">
+        <v>113.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>78</v>
+      </c>
+      <c r="B60">
+        <v>113.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>79</v>
+      </c>
+      <c r="B61">
+        <v>113.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>80</v>
+      </c>
+      <c r="B62">
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>81</v>
+      </c>
+      <c r="B63">
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>82</v>
+      </c>
+      <c r="B64">
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>83</v>
+      </c>
+      <c r="B65">
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>84</v>
+      </c>
+      <c r="B66">
+        <v>125.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <f>SUM(B2:B66)</f>
+        <v>2931.6499999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="e">
+        <f>B67/C67</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70F1971-0905-427D-AA08-ACCA3854A2E7}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9826,12 +10537,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70545A2-5E38-47E2-9BDE-E0A90D33D650}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11752,7 +12463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43C27B9-84A9-433A-B988-B71729F4368A}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -11990,4 +12701,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E666E5-9F6E-4F37-ADD0-A98CFE1A2C48}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>0.3532934131736527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>0.25449101796407186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>0.39221556886227543</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
US vs DR initial chart in excel
</commit_message>
<xml_diff>
--- a/data/incidence_dr_globocan.xlsx
+++ b/data/incidence_dr_globocan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/st3381_cumc_columbia_edu/Documents/HIRE/CRC Screening Models/dr-crc-calibration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="330" documentId="8_{35A0E001-2FA2-487A-9E36-68090B21B923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B72A00FB-0FBB-4EE4-9067-DA6D58856CB9}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="8_{35A0E001-2FA2-487A-9E36-68090B21B923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B19CE22-0EE5-43DE-968E-25C26C7ACFD2}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="34590" yWindow="990" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{28CE8278-F064-480C-86D8-BD239664EDA6}"/>
+    <workbookView xWindow="28680" yWindow="-1875" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{28CE8278-F064-480C-86D8-BD239664EDA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Globocan" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="1Y INC" sheetId="2" r:id="rId3"/>
     <sheet name="DR 5y raw" sheetId="10" r:id="rId4"/>
     <sheet name="DR incidence factor" sheetId="6" r:id="rId5"/>
-    <sheet name="1Y INC US STAGE DIST" sheetId="3" r:id="rId6"/>
-    <sheet name="DR 5y factor" sheetId="4" r:id="rId7"/>
-    <sheet name="HGPS Stage" sheetId="11" r:id="rId8"/>
+    <sheet name="DR globo v seer" sheetId="12" r:id="rId6"/>
+    <sheet name="1Y INC US STAGE DIST" sheetId="3" r:id="rId7"/>
+    <sheet name="DR 5y factor" sheetId="4" r:id="rId8"/>
+    <sheet name="HGPS Stage" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Age</t>
   </si>
@@ -184,6 +185,12 @@
   </si>
   <si>
     <t>Distant</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -3097,6 +3104,1165 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Age-specific incidence</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'DR globo v seer'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DR Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'DR globo v seer'!$A$2:$A$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'DR globo v seer'!$B$2:$B$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0.41081956044171342</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2148070458101218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50283020334105666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81869682800018451</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72161135798559184</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1351618234592933</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0623623924649055</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2261860016440855</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4753106732021559</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8452041198809845</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0908522234015789</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5203799042155417</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.7232275335678389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0976415472978673</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2657408086617288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1308812046460259</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7554059154105888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.899615648197778</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.6307475147847779</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.8453167530663519</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.0393318855910501</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.9680907370773006</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.0167724262334001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.281698313036765</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.786665299533983</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.667521728703967</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15.584049619349651</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18.437122552452973</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21.224364510882282</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21.82363803149525</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24.988144083697325</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28.085315086303776</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.185481986446263</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.928846624672175</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36.358168991894658</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37.676917287071113</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42.251902347202915</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>47.480961050035766</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>52.149924254229994</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>53.491362566245556</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>58.419790136200781</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>61.840690874776818</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>64.84960453233046</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>68.297566900224794</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>70.024520402873009</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>74.442299671306202</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>77.570164278457327</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>81.80876880985025</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>84.172685249154682</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>85.615299812503181</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>91.108271936209846</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>92.636648000970581</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>94.642079925147257</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>98.95757544065907</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>101.85783450443178</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>104.31825184842279</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>105.21024468572486</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>105.30069892706818</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>107.52128254001255</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>107.01506361767574</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>110.93215250322311</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>114.53069093470711</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>108.0986928543667</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>109.25834376831419</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>105.26090821823124</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5EC9-45DA-AB5F-F701CB99F55D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'DR globo v seer'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>US Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'DR globo v seer'!$A$2:$A$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'DR globo v seer'!$C$2:$C$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0.26038792593205357</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13987632135665642</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33638993054339439</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56269193373351722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.50953836956025333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82348797314530864</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79176832406398845</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93887492364599689</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1605418904479927</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4912405462339557</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7360114202843586</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1499145459199647</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3865199562022594</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.7889341010790005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0207498050243307</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.9255607231015919</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.6427204942280955</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.9144272331895724</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.8023363551657132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.2469680560743024</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.7439709657768923</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.021083795738132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.351225260498525</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.12638796235653</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.070125454398427</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17.014072420318239</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19.930802121463909</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24.224986769430302</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.650423950307431</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.265611838691196</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35.602644727407736</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41.110571165761293</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>48.401651273215101</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>53.964773338854748</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>57.710397682350425</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>61.44030683274481</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>70.786466282319353</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>81.72396271572039</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>92.216694126404647</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>97.177445559538</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>109.03546039956781</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>118.57907358242832</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>127.75179271980907</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>138.22635453791031</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>145.60011442456053</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>159.02203439387833</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>170.23865776851429</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>184.45451196947829</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>194.978425672394</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>203.7476977697734</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>222.75378319003488</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>232.68911205000498</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>244.23250138464721</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>262.35791960495698</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>277.43772987697616</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>291.91562058647429</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>302.46910135425475</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>311.01418002202342</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>326.26412559849217</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>333.61514078162958</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>355.29101889593704</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>376.85529453457707</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>365.42573898390043</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>379.45410485115463</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>375.57589114137124</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5EC9-45DA-AB5F-F701CB99F55D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="162975648"/>
+        <c:axId val="162976128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="162975648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="162976128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="162976128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="162975648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3178,6 +4344,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4765,6 +5971,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4878,6 +6600,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07EF6A3B-27C4-81D9-971C-FAC1802E67DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5657,7 +7420,7 @@
   <dimension ref="A1:V68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9349,8 +11112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70F1971-0905-427D-AA08-ACCA3854A2E7}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10538,6 +12301,772 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B5A134-78B1-43E8-9828-56C58E37F40D}">
+  <dimension ref="A1:E67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0.41081956044171342</v>
+      </c>
+      <c r="C2">
+        <v>0.26038792593205357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>0.2148070458101218</v>
+      </c>
+      <c r="C3">
+        <v>0.13987632135665642</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>0.50283020334105666</v>
+      </c>
+      <c r="C4">
+        <v>0.33638993054339439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>0.81869682800018451</v>
+      </c>
+      <c r="C5">
+        <v>0.56269193373351722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0.72161135798559184</v>
+      </c>
+      <c r="C6">
+        <v>0.50953836956025333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>1.1351618234592933</v>
+      </c>
+      <c r="C7">
+        <v>0.82348797314530864</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1.0623623924649055</v>
+      </c>
+      <c r="C8">
+        <v>0.79176832406398845</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>1.2261860016440855</v>
+      </c>
+      <c r="C9">
+        <v>0.93887492364599689</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>1.4753106732021559</v>
+      </c>
+      <c r="C10">
+        <v>1.1605418904479927</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>1.8452041198809845</v>
+      </c>
+      <c r="C11">
+        <v>1.4912405462339557</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>2.0908522234015789</v>
+      </c>
+      <c r="C12">
+        <v>1.7360114202843586</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>2.5203799042155417</v>
+      </c>
+      <c r="C13">
+        <v>2.1499145459199647</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>2.7232275335678389</v>
+      </c>
+      <c r="C14">
+        <v>2.3865199562022594</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>3.0976415472978673</v>
+      </c>
+      <c r="C15">
+        <v>2.7889341010790005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>3.2657408086617288</v>
+      </c>
+      <c r="C16">
+        <v>3.0207498050243307</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>4.1308812046460259</v>
+      </c>
+      <c r="C17">
+        <v>3.9255607231015919</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>4.7554059154105888</v>
+      </c>
+      <c r="C18">
+        <v>4.6427204942280955</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>37</v>
+      </c>
+      <c r="B19">
+        <v>4.899615648197778</v>
+      </c>
+      <c r="C19">
+        <v>4.9144272331895724</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>38</v>
+      </c>
+      <c r="B20">
+        <v>5.6307475147847779</v>
+      </c>
+      <c r="C20">
+        <v>5.8023363551657132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>6.8453167530663519</v>
+      </c>
+      <c r="C21">
+        <v>7.2469680560743024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <v>8.0393318855910501</v>
+      </c>
+      <c r="C22">
+        <v>8.7439709657768923</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>8.9680907370773006</v>
+      </c>
+      <c r="C23">
+        <v>10.021083795738132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>9.0167724262334001</v>
+      </c>
+      <c r="C24">
+        <v>10.351225260498525</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>10.281698313036765</v>
+      </c>
+      <c r="C25">
+        <v>12.12638796235653</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>44</v>
+      </c>
+      <c r="B26">
+        <v>10.786665299533983</v>
+      </c>
+      <c r="C26">
+        <v>13.070125454398427</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>45</v>
+      </c>
+      <c r="B27">
+        <v>13.667521728703967</v>
+      </c>
+      <c r="C27">
+        <v>17.014072420318239</v>
+      </c>
+      <c r="D27">
+        <f>B27/B62</f>
+        <v>0.12320613474354841</v>
+      </c>
+      <c r="E27">
+        <f>C27/C62</f>
+        <v>4.7887707584585965E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>46</v>
+      </c>
+      <c r="B28">
+        <v>15.584049619349651</v>
+      </c>
+      <c r="C28">
+        <v>19.930802121463909</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>18.437122552452973</v>
+      </c>
+      <c r="C29">
+        <v>24.224986769430302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>48</v>
+      </c>
+      <c r="B30">
+        <v>21.224364510882282</v>
+      </c>
+      <c r="C30">
+        <v>28.650423950307431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>49</v>
+      </c>
+      <c r="B31">
+        <v>21.82363803149525</v>
+      </c>
+      <c r="C31">
+        <v>30.265611838691196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>50</v>
+      </c>
+      <c r="B32">
+        <v>24.988144083697325</v>
+      </c>
+      <c r="C32">
+        <v>35.602644727407736</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>51</v>
+      </c>
+      <c r="B33">
+        <v>28.085315086303776</v>
+      </c>
+      <c r="C33">
+        <v>41.110571165761293</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <v>32.185481986446263</v>
+      </c>
+      <c r="C34">
+        <v>48.401651273215101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>34.928846624672175</v>
+      </c>
+      <c r="C35">
+        <v>53.964773338854748</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>54</v>
+      </c>
+      <c r="B36">
+        <v>36.358168991894658</v>
+      </c>
+      <c r="C36">
+        <v>57.710397682350425</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>55</v>
+      </c>
+      <c r="B37">
+        <v>37.676917287071113</v>
+      </c>
+      <c r="C37">
+        <v>61.44030683274481</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>56</v>
+      </c>
+      <c r="B38">
+        <v>42.251902347202915</v>
+      </c>
+      <c r="C38">
+        <v>70.786466282319353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>47.480961050035766</v>
+      </c>
+      <c r="C39">
+        <v>81.72396271572039</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>58</v>
+      </c>
+      <c r="B40">
+        <v>52.149924254229994</v>
+      </c>
+      <c r="C40">
+        <v>92.216694126404647</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>59</v>
+      </c>
+      <c r="B41">
+        <v>53.491362566245556</v>
+      </c>
+      <c r="C41">
+        <v>97.177445559538</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>60</v>
+      </c>
+      <c r="B42">
+        <v>58.419790136200781</v>
+      </c>
+      <c r="C42">
+        <v>109.03546039956781</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>61</v>
+      </c>
+      <c r="B43">
+        <v>61.840690874776818</v>
+      </c>
+      <c r="C43">
+        <v>118.57907358242832</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>62</v>
+      </c>
+      <c r="B44">
+        <v>64.84960453233046</v>
+      </c>
+      <c r="C44">
+        <v>127.75179271980907</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>63</v>
+      </c>
+      <c r="B45">
+        <v>68.297566900224794</v>
+      </c>
+      <c r="C45">
+        <v>138.22635453791031</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>64</v>
+      </c>
+      <c r="B46">
+        <v>70.024520402873009</v>
+      </c>
+      <c r="C46">
+        <v>145.60011442456053</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>65</v>
+      </c>
+      <c r="B47">
+        <v>74.442299671306202</v>
+      </c>
+      <c r="C47">
+        <v>159.02203439387833</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>66</v>
+      </c>
+      <c r="B48">
+        <v>77.570164278457327</v>
+      </c>
+      <c r="C48">
+        <v>170.23865776851429</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>67</v>
+      </c>
+      <c r="B49">
+        <v>81.80876880985025</v>
+      </c>
+      <c r="C49">
+        <v>184.45451196947829</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>68</v>
+      </c>
+      <c r="B50">
+        <v>84.172685249154682</v>
+      </c>
+      <c r="C50">
+        <v>194.978425672394</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>69</v>
+      </c>
+      <c r="B51">
+        <v>85.615299812503181</v>
+      </c>
+      <c r="C51">
+        <v>203.7476977697734</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>70</v>
+      </c>
+      <c r="B52">
+        <v>91.108271936209846</v>
+      </c>
+      <c r="C52">
+        <v>222.75378319003488</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>71</v>
+      </c>
+      <c r="B53">
+        <v>92.636648000970581</v>
+      </c>
+      <c r="C53">
+        <v>232.68911205000498</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>72</v>
+      </c>
+      <c r="B54">
+        <v>94.642079925147257</v>
+      </c>
+      <c r="C54">
+        <v>244.23250138464721</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>73</v>
+      </c>
+      <c r="B55">
+        <v>98.95757544065907</v>
+      </c>
+      <c r="C55">
+        <v>262.35791960495698</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>74</v>
+      </c>
+      <c r="B56">
+        <v>101.85783450443178</v>
+      </c>
+      <c r="C56">
+        <v>277.43772987697616</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>75</v>
+      </c>
+      <c r="B57">
+        <v>104.31825184842279</v>
+      </c>
+      <c r="C57">
+        <v>291.91562058647429</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>76</v>
+      </c>
+      <c r="B58">
+        <v>105.21024468572486</v>
+      </c>
+      <c r="C58">
+        <v>302.46910135425475</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>77</v>
+      </c>
+      <c r="B59">
+        <v>105.30069892706818</v>
+      </c>
+      <c r="C59">
+        <v>311.01418002202342</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>78</v>
+      </c>
+      <c r="B60">
+        <v>107.52128254001255</v>
+      </c>
+      <c r="C60">
+        <v>326.26412559849217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>79</v>
+      </c>
+      <c r="B61">
+        <v>107.01506361767574</v>
+      </c>
+      <c r="C61">
+        <v>333.61514078162958</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>80</v>
+      </c>
+      <c r="B62">
+        <v>110.93215250322311</v>
+      </c>
+      <c r="C62">
+        <v>355.29101889593704</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>81</v>
+      </c>
+      <c r="B63">
+        <v>114.53069093470711</v>
+      </c>
+      <c r="C63">
+        <v>376.85529453457707</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>82</v>
+      </c>
+      <c r="B64">
+        <v>108.0986928543667</v>
+      </c>
+      <c r="C64">
+        <v>365.42573898390043</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>83</v>
+      </c>
+      <c r="B65">
+        <v>109.25834376831419</v>
+      </c>
+      <c r="C65">
+        <v>379.45410485115463</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>84</v>
+      </c>
+      <c r="B66">
+        <v>105.26090821823124</v>
+      </c>
+      <c r="C66">
+        <v>375.57589114137124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <f t="shared" ref="B67" si="0">SUM(B2:B66)</f>
+        <v>2860.4892088144793</v>
+      </c>
+      <c r="C67">
+        <f>SUM(C2:C66)</f>
+        <v>7069.1479311669773</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70545A2-5E38-47E2-9BDE-E0A90D33D650}">
   <dimension ref="A1:H66"/>
   <sheetViews>
@@ -12463,7 +14992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43C27B9-84A9-433A-B988-B71729F4368A}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -12703,7 +15232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E666E5-9F6E-4F37-ADD0-A98CFE1A2C48}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>